<commit_message>
profit and loss account
</commit_message>
<xml_diff>
--- a/01 Accounting Equation.xlsx
+++ b/01 Accounting Equation.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mr Hoang\01Marketing\01Accounting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259AA2DB-D245-4549-9861-A638383CA999}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C70E96-0186-4542-AD3C-0B6F4E71E724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="1710" windowWidth="18450" windowHeight="9675" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="765" windowWidth="18450" windowHeight="9675" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Balance" sheetId="3" r:id="rId3"/>
+    <sheet name="Profit_Loss_Account" sheetId="4" r:id="rId4"/>
+    <sheet name="Debit_Credit_Rules" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,8 +34,46 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Nguyen Ngoc Hoang</author>
+  </authors>
+  <commentList>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{A1A0692A-F2E2-4871-A386-08C6AFE06516}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nguyen Ngoc Hoang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+OK so let's take a look at balance sheet balance sheet is the most important report in any business
+and the key purpose of accounting is to prepared the two main reports.
+One is balance sheet and advance profit and loss account that we will be looking at in a while.
+So in balance sheet.
+First of all you will have a summary of assets.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="99">
   <si>
     <t>Assets = Liabilities + Capital</t>
   </si>
@@ -195,13 +235,155 @@
   </si>
   <si>
     <t>TOTAL Liabilities and owner's equity</t>
+  </si>
+  <si>
+    <t>YOUR COMPANY</t>
+  </si>
+  <si>
+    <t>Company Name
+Profit &amp; Loss Statement
+For the year ended 31 Dec 2019</t>
+  </si>
+  <si>
+    <t>Prior Period</t>
+  </si>
+  <si>
+    <t>Current Period</t>
+  </si>
+  <si>
+    <t>Sales Revenue</t>
+  </si>
+  <si>
+    <t>Product/Service 1</t>
+  </si>
+  <si>
+    <t>Product/Service 2</t>
+  </si>
+  <si>
+    <t>Product/Service 3</t>
+  </si>
+  <si>
+    <t>Product/Service 4</t>
+  </si>
+  <si>
+    <t>Cost of Sales</t>
+  </si>
+  <si>
+    <t>Total Sales Revenue [J]:</t>
+  </si>
+  <si>
+    <t>Total Cost of Sales [K]:</t>
+  </si>
+  <si>
+    <t>Gross Profit [L] = [J] - [K]</t>
+  </si>
+  <si>
+    <t>Operating Expenses</t>
+  </si>
+  <si>
+    <t>Sales and Marketing</t>
+  </si>
+  <si>
+    <t>Advertsing</t>
+  </si>
+  <si>
+    <t>Direct marketing</t>
+  </si>
+  <si>
+    <t>Other expenses (specify)</t>
+  </si>
+  <si>
+    <t>Total Sales and Marketing
+Expenses [M]</t>
+  </si>
+  <si>
+    <t>Research and Development</t>
+  </si>
+  <si>
+    <t>Technology licenses</t>
+  </si>
+  <si>
+    <t>Patents</t>
+  </si>
+  <si>
+    <t>Total  Research and
+Development Expenses [N]</t>
+  </si>
+  <si>
+    <t>General and Administrative</t>
+  </si>
+  <si>
+    <t>Wages and salaries</t>
+  </si>
+  <si>
+    <t>Outside services</t>
+  </si>
+  <si>
+    <t>Supplies</t>
+  </si>
+  <si>
+    <t>Meals and entertainment</t>
+  </si>
+  <si>
+    <t>Rent</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Depreciation</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Repairs and maintanance</t>
+  </si>
+  <si>
+    <t>Total  General and Administrative Expenses [O]</t>
+  </si>
+  <si>
+    <t>Total Operating Expenses
+ [P] = [M] + [N] + [0]</t>
+  </si>
+  <si>
+    <t>Income from Operations
+ [Q] = [L] - [P]</t>
+  </si>
+  <si>
+    <t>Other Income [R]</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>Income taxes</t>
+  </si>
+  <si>
+    <t>Payroll taxes</t>
+  </si>
+  <si>
+    <t>Real estaste taxes</t>
+  </si>
+  <si>
+    <t>Other taxes (specify)</t>
+  </si>
+  <si>
+    <t>Total Taxes [S]:</t>
+  </si>
+  <si>
+    <t>Net Profit
+ [T] = [Q + R - S]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,8 +440,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,8 +520,24 @@
         <fgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -351,37 +590,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="6"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="9">
+    <cellStyle name="40% - Accent5" xfId="8" builtinId="47"/>
+    <cellStyle name="Accent5" xfId="7" builtinId="45"/>
     <cellStyle name="Accent6" xfId="5" builtinId="49"/>
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="4" builtinId="10"/>
+    <cellStyle name="Output" xfId="6" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -661,9 +957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -873,15 +1167,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="F2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="2:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
@@ -951,11 +1245,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD47E618-20EC-4370-A264-D7199E3E8044}">
-  <dimension ref="A2:C44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD47E618-20EC-4370-A264-D7199E3E8044}">
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,281 +1259,287 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="23" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A23" s="7" t="s">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+    </row>
+    <row r="24" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A24" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A25" s="7" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A26" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C36" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C40" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-    </row>
-    <row r="44" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A44" s="7" t="s">
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+    </row>
+    <row r="45" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A45" s="6" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3">
+  <conditionalFormatting sqref="A4">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1251,7 +1551,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
+  <conditionalFormatting sqref="A13">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1263,7 +1563,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A19">
+  <conditionalFormatting sqref="A20">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1275,7 +1575,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A26">
+  <conditionalFormatting sqref="A27">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1287,7 +1587,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A35">
+  <conditionalFormatting sqref="A36">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1299,7 +1599,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39">
+  <conditionalFormatting sqref="A40">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1313,5 +1613,422 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D712B1-3139-4F6A-A854-E595B9023238}">
+  <dimension ref="A1:C63"/>
+  <sheetViews>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="3" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+    </row>
+    <row r="12" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+    </row>
+    <row r="21" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A21" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+    </row>
+    <row r="22" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+    </row>
+    <row r="27" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+    </row>
+    <row r="28" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A28" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+    </row>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+    </row>
+    <row r="34" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A34" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="19"/>
+      <c r="C34" s="20"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+    </row>
+    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+    </row>
+    <row r="49" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
+    </row>
+    <row r="53" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+    </row>
+    <row r="55" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A55" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="C55" s="14"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
+    </row>
+    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B63" s="23"/>
+      <c r="C63" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64ED17D9-BB1F-4EFD-BF97-4537258E85C7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
debit and credit rule
</commit_message>
<xml_diff>
--- a/01 Accounting Equation.xlsx
+++ b/01 Accounting Equation.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mr Hoang\01Marketing\01Accounting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01Sach\Business\BookkeepingAccountingFinancialStatements\01Accounting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C70E96-0186-4542-AD3C-0B6F4E71E724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="765" windowWidth="18450" windowHeight="9675" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2508" yWindow="768" windowWidth="18456" windowHeight="9672" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Assets" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="Profit_Loss_Account" sheetId="4" r:id="rId4"/>
     <sheet name="Debit_Credit_Rules" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,12 +34,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyen Ngoc Hoang</author>
   </authors>
   <commentList>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{A1A0692A-F2E2-4871-A386-08C6AFE06516}">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -73,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="103">
   <si>
     <t>Assets = Liabilities + Capital</t>
   </si>
@@ -377,12 +376,24 @@
   <si>
     <t>Net Profit
  [T] = [Q + R - S]</t>
+  </si>
+  <si>
+    <t>Debit</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Increase</t>
+  </si>
+  <si>
+    <t>decrease</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -537,7 +548,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -614,6 +625,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -626,7 +657,7 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -637,9 +668,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -653,9 +681,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
@@ -667,6 +692,14 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="8" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="40% - Accent5" xfId="8" builtinId="47"/>
@@ -954,20 +987,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -975,7 +1008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -986,7 +1019,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B3" s="1">
         <v>0</v>
       </c>
@@ -997,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1009,7 +1042,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1021,7 +1054,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1032,7 +1065,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1044,7 +1077,7 @@
         <v>-200</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1055,7 +1088,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B9" s="2">
         <f>SUM(B4:B8)</f>
         <v>1300</v>
@@ -1069,7 +1102,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1084,7 +1117,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1099,7 +1132,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1114,7 +1147,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1129,7 +1162,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B15" s="2">
         <f>SUM(B9:B14)</f>
         <v>1670</v>
@@ -1150,34 +1183,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD248F2-5B63-4404-918D-61082D2D1BBD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="F2" s="10" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="F2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="2:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="G2" s="22"/>
+    </row>
+    <row r="3" spans="2:8" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1197,7 +1230,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
         <v>18</v>
       </c>
@@ -1245,32 +1278,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD47E618-20EC-4370-A264-D7199E3E8044}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="59" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:7" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -1281,56 +1314,56 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
@@ -1341,42 +1374,42 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>34</v>
       </c>
@@ -1387,36 +1420,36 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
     </row>
-    <row r="24" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A24" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A26" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>39</v>
       </c>
@@ -1427,56 +1460,56 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>45</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
         <v>46</v>
       </c>
@@ -1487,21 +1520,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
         <v>49</v>
       </c>
@@ -1512,28 +1545,28 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
     </row>
-    <row r="45" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A45" s="6" t="s">
         <v>53</v>
       </c>
@@ -1618,391 +1651,391 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D712B1-3139-4F6A-A854-E595B9023238}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
       <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:3" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-    </row>
-    <row r="3" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+    </row>
+    <row r="3" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-    </row>
-    <row r="12" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="12" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A12" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-    </row>
-    <row r="21" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+    </row>
+    <row r="21" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A21" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-    </row>
-    <row r="22" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A22" s="21" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+    </row>
+    <row r="22" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A22" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-    </row>
-    <row r="27" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-    </row>
-    <row r="28" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A28" s="21" t="s">
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+    </row>
+    <row r="28" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A28" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="20"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
+      <c r="B28" s="17"/>
+      <c r="C28" s="18"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-    </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-    </row>
-    <row r="34" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A34" s="21" t="s">
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+    </row>
+    <row r="34" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A34" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="20"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="15"/>
-      <c r="C42" s="15"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-    </row>
-    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="s">
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+    </row>
+    <row r="47" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-    </row>
-    <row r="49" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22" t="s">
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+    </row>
+    <row r="49" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-    </row>
-    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="s">
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+    </row>
+    <row r="51" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
-    </row>
-    <row r="53" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+    </row>
+    <row r="53" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="B53" s="23"/>
-      <c r="C53" s="23"/>
-    </row>
-    <row r="55" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A55" s="13" t="s">
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+    </row>
+    <row r="55" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A55" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B55" s="13"/>
-      <c r="C55" s="14"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
+      <c r="B55" s="12"/>
+      <c r="C55" s="13"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="12" t="s">
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="15"/>
-      <c r="C58" s="15"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="12" t="s">
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B60" s="15"/>
-      <c r="C60" s="15"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
-    </row>
-    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="22" t="s">
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+    </row>
+    <row r="63" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="B63" s="23"/>
-      <c r="C63" s="23"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2014,21 +2047,100 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64ED17D9-BB1F-4EFD-BF97-4537258E85C7}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="G5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="E7" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="25"/>
+      <c r="G8" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" s="25"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="H9" s="25"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>